<commit_message>
Fixing errors in Lab 02
</commit_message>
<xml_diff>
--- a/02_av_fistula/02_av_fistula_data.xlsx
+++ b/02_av_fistula/02_av_fistula_data.xlsx
@@ -16,7 +16,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+  <si>
+    <t>A-V Fistula Data</t>
+  </si>
   <si>
     <t>Time</t>
   </si>
@@ -82,6 +85,54 @@
   </si>
   <si>
     <t>Hematocrit(%)</t>
+  </si>
+  <si>
+    <t>1-Month Exercise results</t>
+  </si>
+  <si>
+    <t>0’</t>
+  </si>
+  <si>
+    <t>1’</t>
+  </si>
+  <si>
+    <t>2’</t>
+  </si>
+  <si>
+    <t>3’</t>
+  </si>
+  <si>
+    <t>4’</t>
+  </si>
+  <si>
+    <t>5’</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Heart Rate</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Distance Traveled</t>
+  </si>
+  <si>
+    <t>Time Elapsed</t>
+  </si>
+  <si>
+    <t>40 seconds</t>
+  </si>
+  <si>
+    <t>0 feet</t>
+  </si>
+  <si>
+    <t>Venous O2 Data and the Fistula</t>
   </si>
   <si>
     <t>Fistula Size</t>
@@ -141,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -159,6 +210,21 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -170,6 +236,19 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -201,24 +280,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -515,364 +606,461 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J7"/>
+      <selection activeCell="P2" sqref="P2:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="30.75" thickBot="1">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C2" s="1">
         <v>10</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="H2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="K2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="30.75" thickBot="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="60.75" thickBot="1">
-      <c r="A3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
-        <v>96.2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>74.2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>75.099999999999994</v>
-      </c>
-      <c r="E3" s="4">
-        <v>72.8</v>
-      </c>
-      <c r="F3" s="4">
-        <v>84.7</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="4">
-        <v>74</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="75.75" thickBot="1">
+        <v>30</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>6</v>
+      </c>
+      <c r="K3" s="2">
+        <v>6</v>
+      </c>
+      <c r="L3" s="2">
+        <v>6</v>
+      </c>
+      <c r="M3" s="2">
+        <v>6</v>
+      </c>
+      <c r="N3" s="2">
+        <v>6</v>
+      </c>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="60.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>5361</v>
+        <v>96</v>
       </c>
       <c r="C4" s="4">
-        <v>7050</v>
+        <v>74</v>
       </c>
       <c r="D4" s="4">
-        <v>6783</v>
+        <v>75</v>
       </c>
       <c r="E4" s="4">
-        <v>7435</v>
-      </c>
-      <c r="F4" s="4">
-        <v>9010</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F4" s="4"/>
       <c r="H4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="4">
-        <v>78</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="45.75" thickBot="1">
+        <v>31</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>74</v>
+      </c>
+      <c r="R4" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="75.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4">
-        <v>72</v>
+        <v>5361</v>
       </c>
       <c r="C5" s="4">
-        <v>85</v>
+        <v>7050</v>
       </c>
       <c r="D5" s="4">
+        <v>6802</v>
+      </c>
+      <c r="E5" s="4">
+        <v>7442</v>
+      </c>
+      <c r="F5" s="4">
+        <v>9019</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="4">
+        <v>79</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="4">
         <v>78</v>
       </c>
-      <c r="E5" s="4">
-        <v>71</v>
-      </c>
-      <c r="F5" s="4">
-        <v>70</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="4">
-        <v>80</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="R5" s="4">
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45.75" thickBot="1">
+    <row r="6" spans="1:18" ht="45.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="4">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D6" s="4">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E6" s="4">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F6" s="4">
-        <v>129</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="4">
-        <v>82</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="45.75" thickBot="1">
+        <v>70</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>80</v>
+      </c>
+      <c r="R6" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="45.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="C7" s="4">
-        <v>3090</v>
+        <v>83</v>
       </c>
       <c r="D7" s="4">
-        <v>3134</v>
+        <v>87</v>
       </c>
       <c r="E7" s="4">
-        <v>3297</v>
+        <v>104</v>
       </c>
       <c r="F7" s="4">
-        <v>3796</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="4">
-        <v>84</v>
-      </c>
-      <c r="J7" s="4">
+        <v>129</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>82</v>
+      </c>
+      <c r="R7" s="4">
         <v>0.17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="60.75" thickBot="1">
+    <row r="8" spans="1:18" ht="60.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="4">
-        <v>845</v>
+        <v>0</v>
       </c>
       <c r="C8" s="4">
-        <v>664</v>
+        <v>3090</v>
       </c>
       <c r="D8" s="4">
-        <v>657</v>
+        <v>3143</v>
       </c>
       <c r="E8" s="4">
-        <v>633</v>
+        <v>3293</v>
       </c>
       <c r="F8" s="4">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="60.75" thickBot="1">
+        <v>3791</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>84</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="60.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="4">
-        <v>975</v>
+        <v>845</v>
       </c>
       <c r="C9" s="4">
-        <v>687</v>
+        <v>664</v>
       </c>
       <c r="D9" s="4">
-        <v>648</v>
+        <v>659</v>
       </c>
       <c r="E9" s="4">
-        <v>803</v>
+        <v>634</v>
       </c>
       <c r="F9" s="4">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="60.75" thickBot="1">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="60.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="4">
-        <v>1185</v>
+        <v>975</v>
       </c>
       <c r="C10" s="4">
-        <v>887</v>
+        <v>688</v>
       </c>
       <c r="D10" s="4">
-        <v>701</v>
+        <v>649</v>
       </c>
       <c r="E10" s="4">
-        <v>774</v>
+        <v>803</v>
       </c>
       <c r="F10" s="4">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="60.75" thickBot="1">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="60.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4">
-        <v>631</v>
+        <v>1185</v>
       </c>
       <c r="C11" s="4">
-        <v>442</v>
+        <v>887</v>
       </c>
       <c r="D11" s="4">
-        <v>414</v>
+        <v>703</v>
       </c>
       <c r="E11" s="4">
-        <v>472</v>
+        <v>777</v>
       </c>
       <c r="F11" s="4">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="45.75" thickBot="1">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="60.75" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="4">
-        <v>1.5</v>
+        <v>631</v>
       </c>
       <c r="C12" s="4">
-        <v>2</v>
+        <v>442</v>
       </c>
       <c r="D12" s="4">
-        <v>1.7</v>
+        <v>415</v>
       </c>
       <c r="E12" s="4">
-        <v>1.5</v>
+        <v>472</v>
       </c>
       <c r="F12" s="4">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="75.75" thickBot="1">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="45.75" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="C13" s="4">
         <v>2</v>
       </c>
-      <c r="C13" s="4">
+      <c r="D13" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="75.75" thickBot="1">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4">
         <v>2.7</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D14" s="4">
         <v>8.5</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E14" s="4">
         <v>2.4</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F14" s="4">
         <v>1.6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="44.25" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5">
+    <row r="15" spans="1:18" ht="60.75" thickBot="1">
+      <c r="A15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4">
         <v>0.12</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C15" s="4">
         <v>0.01</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D15" s="4">
         <v>0</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E15" s="4">
         <v>0.08</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F15" s="4">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" ht="45.75" thickBot="1">
+    <row r="16" spans="1:18" ht="45.75" thickBot="1">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" s="4">
         <v>19</v>
@@ -887,12 +1075,12 @@
         <v>19</v>
       </c>
       <c r="F16" s="4">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45.75" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="4">
         <v>5400</v>
@@ -904,15 +1092,15 @@
         <v>5415</v>
       </c>
       <c r="E17" s="4">
-        <v>5958</v>
+        <v>5956</v>
       </c>
       <c r="F17" s="4">
-        <v>6169</v>
+        <v>6168</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60.75" thickBot="1">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" s="4">
         <v>2400</v>
@@ -924,15 +1112,15 @@
         <v>2400</v>
       </c>
       <c r="E18" s="4">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="F18" s="4">
-        <v>2540</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45.75" thickBot="1">
       <c r="A19" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" s="4">
         <v>3000</v>
@@ -944,15 +1132,15 @@
         <v>3016</v>
       </c>
       <c r="E19" s="4">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="F19" s="4">
-        <v>3629</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30.75" thickBot="1">
       <c r="A20" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" s="4">
         <v>44</v>
@@ -971,15 +1159,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="P2:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixing Lab 2 charts
</commit_message>
<xml_diff>
--- a/02_av_fistula/02_av_fistula_data.xlsx
+++ b/02_av_fistula/02_av_fistula_data.xlsx
@@ -312,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -358,9 +358,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -373,13 +370,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -405,69 +412,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -770,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:F63"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="V55" sqref="V55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -794,7 +738,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="30.75" thickBot="1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -833,7 +777,7 @@
       <c r="N2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="17" t="s">
         <v>37</v>
       </c>
       <c r="Q2" s="1" t="s">
@@ -844,7 +788,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="30.75" thickBot="1">
-      <c r="A3" s="19"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -881,7 +825,7 @@
       <c r="N3" s="2">
         <v>6</v>
       </c>
-      <c r="P3" s="19"/>
+      <c r="P3" s="18"/>
       <c r="Q3" s="2" t="s">
         <v>39</v>
       </c>
@@ -1343,7 +1287,7 @@
       </c>
     </row>
     <row r="24" spans="1:36" ht="30.75" thickBot="1">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="1">
@@ -1382,7 +1326,7 @@
       <c r="N24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P24" s="18" t="s">
+      <c r="P24" s="17" t="s">
         <v>37</v>
       </c>
       <c r="Q24" s="1" t="s">
@@ -1393,7 +1337,7 @@
       </c>
     </row>
     <row r="25" spans="1:36" ht="30.75" thickBot="1">
-      <c r="A25" s="19"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
@@ -1430,7 +1374,7 @@
       <c r="N25" s="2">
         <v>6</v>
       </c>
-      <c r="P25" s="19"/>
+      <c r="P25" s="18"/>
       <c r="Q25" s="2" t="s">
         <v>39</v>
       </c>
@@ -1700,13 +1644,13 @@
       <c r="F32" s="4">
         <v>832</v>
       </c>
-      <c r="H32" s="20" t="s">
+      <c r="H32" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
     </row>
     <row r="33" spans="1:18" ht="60.75" thickBot="1">
       <c r="A33" s="10" t="s">
@@ -1727,11 +1671,11 @@
       <c r="F33" s="4">
         <v>951</v>
       </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
     </row>
     <row r="34" spans="1:18" ht="60.75" thickBot="1">
       <c r="A34" s="10" t="s">
@@ -1919,618 +1863,620 @@
       </c>
     </row>
     <row r="45" spans="1:18" ht="30.75" thickBot="1">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="22">
         <v>0</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="22">
         <v>10</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="22">
         <v>1</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="22">
         <v>1</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="22">
         <v>1</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I45" s="6" t="s">
+      <c r="I45" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J45" s="6" t="s">
+      <c r="J45" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="6" t="s">
+      <c r="K45" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="L45" s="6" t="s">
+      <c r="L45" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="M45" s="6" t="s">
+      <c r="M45" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="N45" s="6" t="s">
+      <c r="N45" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="P45" s="18" t="s">
+      <c r="P45" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="Q45" s="1" t="s">
+      <c r="Q45" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="R45" s="1" t="s">
+      <c r="R45" s="22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="30.75" thickBot="1">
-      <c r="A46" s="19"/>
-      <c r="B46" s="2" t="s">
+      <c r="A46" s="21"/>
+      <c r="B46" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="22">
         <v>0</v>
       </c>
-      <c r="J46" s="2">
+      <c r="J46" s="22">
         <v>6</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="22">
         <v>6</v>
       </c>
-      <c r="L46" s="2">
+      <c r="L46" s="22">
         <v>6</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M46" s="22">
         <v>6</v>
       </c>
-      <c r="N46" s="2">
+      <c r="N46" s="22">
         <v>6</v>
       </c>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="2" t="s">
+      <c r="P46" s="21"/>
+      <c r="Q46" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="R46" s="2" t="s">
+      <c r="R46" s="22" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="23">
         <f>ABS((B4-B26)/B4)*100</f>
         <v>0.41237113402062436</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="24">
         <f>ABS((C4-C26)/C4)</f>
         <v>2.1052631578947295E-2</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="24">
         <f t="shared" ref="D47:F47" si="0">ABS((D4-D26)/D4)</f>
         <v>5.2631578947368418E-2</v>
       </c>
-      <c r="E47" s="22">
+      <c r="E47" s="24">
         <f t="shared" si="0"/>
         <v>4.3835616438356206E-2</v>
       </c>
-      <c r="F47" s="22">
+      <c r="F47" s="24">
         <f t="shared" si="0"/>
         <v>2.3170731707317142E-2</v>
       </c>
-      <c r="H47" s="17" t="s">
+      <c r="H47" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I47" s="7">
+      <c r="I47" s="25">
         <v>0</v>
       </c>
-      <c r="J47" s="7">
+      <c r="J47" s="25">
         <v>0</v>
       </c>
-      <c r="K47" s="7">
+      <c r="K47" s="25">
         <v>0.02</v>
       </c>
-      <c r="L47" s="7">
+      <c r="L47" s="25">
         <v>0.04</v>
       </c>
-      <c r="M47" s="7">
+      <c r="M47" s="25">
         <v>0.06</v>
       </c>
-      <c r="N47" s="7">
+      <c r="N47" s="25">
         <v>0.08</v>
       </c>
-      <c r="P47" s="17" t="s">
+      <c r="P47" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Q47" s="22">
+      <c r="Q47" s="24">
         <f>ABS((Q4-Q26)/Q4)</f>
         <v>1.466666666666659E-2</v>
       </c>
-      <c r="R47" s="22">
+      <c r="R47" s="24">
         <f>ABS((R4-R26)/R4)</f>
         <v>6.6666666666666732E-3</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B48">
-        <f t="shared" ref="B48:F48" si="1">ABS((B5-B27)/B5)*100</f>
+      <c r="B48" s="23">
+        <f t="shared" ref="B48" si="1">ABS((B5-B27)/B5)*100</f>
         <v>2.2820800598578375</v>
       </c>
-      <c r="C48" s="22">
+      <c r="C48" s="24">
         <f t="shared" ref="C48:F48" si="2">ABS((C5-C27)/C5)</f>
         <v>9.8779612347451543E-2</v>
       </c>
-      <c r="D48" s="22">
+      <c r="D48" s="24">
         <f t="shared" si="2"/>
         <v>6.3021454112038147E-2</v>
       </c>
-      <c r="E48" s="22">
+      <c r="E48" s="24">
         <f t="shared" si="2"/>
         <v>5.7656629085200514E-2</v>
       </c>
-      <c r="F48" s="22">
+      <c r="F48" s="24">
         <f t="shared" si="2"/>
         <v>3.408567480423768E-2</v>
       </c>
-      <c r="H48" s="17" t="s">
+      <c r="H48" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I48" s="22">
+      <c r="I48" s="24">
         <f>ABS((I5-I27)/I5)</f>
         <v>0.15</v>
       </c>
-      <c r="J48" s="22">
+      <c r="J48" s="24">
         <f t="shared" ref="J48:L48" si="3">ABS((J5-J27)/J5)</f>
         <v>2.4E-2</v>
       </c>
-      <c r="K48" s="22">
+      <c r="K48" s="24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L48" s="22">
+      <c r="L48" s="24">
         <f t="shared" si="3"/>
         <v>8.8435374149659865E-2</v>
       </c>
-      <c r="P48" s="17" t="s">
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
+      <c r="P48" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q48" s="22">
+      <c r="Q48" s="24">
         <f t="shared" ref="Q48:R51" si="4">ABS((Q5-Q27)/Q5)</f>
         <v>3.1168831168831242E-2</v>
       </c>
-      <c r="R48" s="22">
+      <c r="R48" s="24">
         <f t="shared" si="4"/>
         <v>2.5000000000000022E-2</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B49">
-        <f t="shared" ref="B49:F49" si="5">ABS((B6-B28)/B6)*100</f>
+      <c r="B49" s="23">
+        <f t="shared" ref="B49" si="5">ABS((B6-B28)/B6)*100</f>
         <v>0</v>
       </c>
-      <c r="C49" s="22">
+      <c r="C49" s="24">
         <f t="shared" ref="C49:F49" si="6">ABS((C6-C28)/C6)</f>
         <v>1.1904761904761904E-2</v>
       </c>
-      <c r="D49" s="22">
+      <c r="D49" s="24">
         <f t="shared" si="6"/>
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="E49" s="22">
+      <c r="E49" s="24">
         <f t="shared" si="6"/>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="F49" s="22">
+      <c r="F49" s="24">
         <f t="shared" si="6"/>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="P49" s="17" t="s">
+      <c r="P49" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q49" s="22">
+      <c r="Q49" s="24">
         <f t="shared" si="4"/>
         <v>3.2499999999999932E-2</v>
       </c>
-      <c r="R49" s="22">
+      <c r="R49" s="24">
         <f t="shared" si="4"/>
         <v>1.2500000000000011E-2</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B50">
-        <f t="shared" ref="B50:F50" si="7">ABS((B7-B29)/B7)*100</f>
+      <c r="B50" s="23">
+        <f t="shared" ref="B50" si="7">ABS((B7-B29)/B7)*100</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="C50" s="22">
+      <c r="C50" s="24">
         <f t="shared" ref="C50:F50" si="8">ABS((C7-C29)/C7)</f>
         <v>0.10843373493975904</v>
       </c>
-      <c r="D50" s="22">
+      <c r="D50" s="24">
         <f t="shared" si="8"/>
         <v>0.12790697674418605</v>
       </c>
-      <c r="E50" s="22">
+      <c r="E50" s="24">
         <f t="shared" si="8"/>
         <v>8.1632653061224483E-2</v>
       </c>
-      <c r="F50" s="22">
+      <c r="F50" s="24">
         <f t="shared" si="8"/>
         <v>2.4193548387096774E-2</v>
       </c>
       <c r="H50" s="11"/>
       <c r="I50" s="9"/>
-      <c r="P50" s="17" t="s">
+      <c r="P50" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q50" s="22">
+      <c r="Q50" s="24">
         <f t="shared" si="4"/>
         <v>4.1463414634146413E-2</v>
       </c>
-      <c r="R50" s="22">
+      <c r="R50" s="24">
         <f t="shared" si="4"/>
         <v>2.3529411764705903E-2</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B51" t="e">
-        <f t="shared" ref="B51:F51" si="9">ABS((B8-B30)/B8)*100</f>
+      <c r="B51" s="23" t="e">
+        <f t="shared" ref="B51" si="9">ABS((B8-B30)/B8)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C51" s="22">
+      <c r="C51" s="24">
         <f t="shared" ref="C51:F51" si="10">ABS((C8-C30)/C8)</f>
         <v>0.12466817740369049</v>
       </c>
-      <c r="D51" s="22">
+      <c r="D51" s="24">
         <f t="shared" si="10"/>
         <v>0.10651817884048471</v>
       </c>
-      <c r="E51" s="22">
+      <c r="E51" s="24">
         <f t="shared" si="10"/>
         <v>0.1048453936882372</v>
       </c>
-      <c r="F51" s="22">
+      <c r="F51" s="24">
         <f t="shared" si="10"/>
         <v>8.9314194577352225E-3</v>
       </c>
       <c r="H51" s="11"/>
       <c r="I51" s="9"/>
-      <c r="P51" s="17" t="s">
+      <c r="P51" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q51" s="22">
+      <c r="Q51" s="24">
         <f t="shared" si="4"/>
         <v>0.12727272727272723</v>
       </c>
-      <c r="R51" s="22">
+      <c r="R51" s="24">
         <f t="shared" si="4"/>
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="60.75" thickBot="1">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B52">
-        <f t="shared" ref="B52:F52" si="11">ABS((B9-B31)/B9)*100</f>
+      <c r="B52" s="23">
+        <f t="shared" ref="B52" si="11">ABS((B9-B31)/B9)*100</f>
         <v>5.3507728894173603</v>
       </c>
-      <c r="C52" s="22">
+      <c r="C52" s="24">
         <f t="shared" ref="C52:F52" si="12">ABS((C9-C31)/C9)</f>
         <v>1.483679525222552E-2</v>
       </c>
-      <c r="D52" s="22">
+      <c r="D52" s="24">
         <f t="shared" si="12"/>
         <v>6.4220183486238536E-2</v>
       </c>
-      <c r="E52" s="22">
+      <c r="E52" s="24">
         <f t="shared" si="12"/>
         <v>0.11937716262975778</v>
       </c>
-      <c r="F52" s="22">
+      <c r="F52" s="24">
         <f t="shared" si="12"/>
         <v>3.8157894736842106E-2</v>
       </c>
     </row>
     <row r="53" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B53">
-        <f t="shared" ref="B53:F53" si="13">ABS((B10-B32)/B10)*100</f>
+      <c r="B53" s="23">
+        <f t="shared" ref="B53" si="13">ABS((B10-B32)/B10)*100</f>
         <v>5.3388090349075972</v>
       </c>
-      <c r="C53" s="22">
+      <c r="C53" s="24">
         <f t="shared" ref="C53:F53" si="14">ABS((C10-C32)/C10)</f>
         <v>9.49367088607595E-2</v>
       </c>
-      <c r="D53" s="22">
+      <c r="D53" s="24">
         <f t="shared" si="14"/>
         <v>3.6392405063291139E-2</v>
       </c>
-      <c r="E53" s="22">
+      <c r="E53" s="24">
         <f t="shared" si="14"/>
         <v>9.3457943925233638E-3</v>
       </c>
-      <c r="F53" s="22">
+      <c r="F53" s="24">
         <f t="shared" si="14"/>
         <v>0.12236286919831224</v>
       </c>
     </row>
     <row r="54" spans="1:18" ht="60.75" thickBot="1">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B54">
-        <f t="shared" ref="B54:F54" si="15">ABS((B11-B33)/B11)*100</f>
+      <c r="B54" s="23">
+        <f t="shared" ref="B54" si="15">ABS((B11-B33)/B11)*100</f>
         <v>3.4367141659681475</v>
       </c>
-      <c r="C54" s="22">
+      <c r="C54" s="24">
         <f t="shared" ref="C54:F54" si="16">ABS((C11-C33)/C11)</f>
         <v>7.7605321507760533E-2</v>
       </c>
-      <c r="D54" s="22">
+      <c r="D54" s="24">
         <f t="shared" si="16"/>
         <v>3.6879432624113473E-2</v>
       </c>
-      <c r="E54" s="22">
+      <c r="E54" s="24">
         <f t="shared" si="16"/>
         <v>2.9609690444145357E-2</v>
       </c>
-      <c r="F54" s="22">
+      <c r="F54" s="24">
         <f t="shared" si="16"/>
         <v>2.922077922077922E-2</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="60.75" thickBot="1">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B55">
-        <f t="shared" ref="B55:F55" si="17">ABS((B12-B34)/B12)*100</f>
+      <c r="B55" s="23">
+        <f t="shared" ref="B55" si="17">ABS((B12-B34)/B12)*100</f>
         <v>25.361155698234349</v>
       </c>
-      <c r="C55" s="22">
+      <c r="C55" s="24">
         <f t="shared" ref="C55:F55" si="18">ABS((C12-C34)/C12)</f>
         <v>0.33488372093023255</v>
       </c>
-      <c r="D55" s="22">
+      <c r="D55" s="24">
         <f t="shared" si="18"/>
         <v>0.23752969121140141</v>
       </c>
-      <c r="E55" s="22">
+      <c r="E55" s="24">
         <f t="shared" si="18"/>
         <v>0.37614678899082571</v>
       </c>
-      <c r="F55" s="22">
+      <c r="F55" s="24">
         <f t="shared" si="18"/>
         <v>0.47533632286995514</v>
       </c>
     </row>
     <row r="56" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B56">
-        <f t="shared" ref="B56:F56" si="19">ABS((B13-B35)/B13)*100</f>
+      <c r="B56" s="23">
+        <f t="shared" ref="B56" si="19">ABS((B13-B35)/B13)*100</f>
         <v>0</v>
       </c>
-      <c r="C56" s="22">
+      <c r="C56" s="24">
         <f t="shared" ref="C56:F56" si="20">ABS((C13-C35)/C13)</f>
         <v>3.0000000000000027E-2</v>
       </c>
-      <c r="D56" s="22">
+      <c r="D56" s="24">
         <f t="shared" si="20"/>
         <v>7.0588235294117577E-2</v>
       </c>
-      <c r="E56" s="22">
+      <c r="E56" s="24">
         <f t="shared" si="20"/>
         <v>6.6666666666666721E-2</v>
       </c>
-      <c r="F56" s="22">
+      <c r="F56" s="24">
         <f t="shared" si="20"/>
         <v>1.4285714285714299E-2</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B57">
-        <f t="shared" ref="B57:F57" si="21">ABS((B14-B36)/B14)*100</f>
+      <c r="B57" s="23">
+        <f t="shared" ref="B57" si="21">ABS((B14-B36)/B14)*100</f>
         <v>10.000000000000009</v>
       </c>
-      <c r="C57" s="22">
+      <c r="C57" s="24">
         <f t="shared" ref="C57:F57" si="22">ABS((C14-C36)/C14)</f>
         <v>3.5714285714285587E-2</v>
       </c>
-      <c r="D57" s="22">
+      <c r="D57" s="24">
         <f t="shared" si="22"/>
         <v>0.25842696629213491</v>
       </c>
-      <c r="E57" s="22">
+      <c r="E57" s="24">
         <f t="shared" si="22"/>
         <v>0.47222222222222227</v>
       </c>
-      <c r="F57" s="22">
+      <c r="F57" s="24">
         <f t="shared" si="22"/>
         <v>0.35294117647058815</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B58">
-        <f t="shared" ref="B58:F58" si="23">ABS((B15-B37)/B15)*100</f>
+      <c r="B58" s="23">
+        <f t="shared" ref="B58" si="23">ABS((B15-B37)/B15)*100</f>
         <v>2.5000000000000022</v>
       </c>
-      <c r="C58" s="22">
+      <c r="C58" s="24">
         <f t="shared" ref="C58:F58" si="24">ABS((C15-C37)/C15)</f>
         <v>1.1999999999999997</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22">
+      <c r="D58" s="24"/>
+      <c r="E58" s="24">
         <f t="shared" si="24"/>
         <v>0.36666666666666664</v>
       </c>
-      <c r="F58" s="22">
+      <c r="F58" s="24">
         <f t="shared" si="24"/>
         <v>0.52307692307692311</v>
       </c>
     </row>
     <row r="59" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A59" s="17" t="s">
+      <c r="A59" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B59">
-        <f t="shared" ref="B59:F59" si="25">ABS((B16-B38)/B16)*100</f>
+      <c r="B59" s="23">
+        <f t="shared" ref="B59" si="25">ABS((B16-B38)/B16)*100</f>
         <v>11.428571428571422</v>
       </c>
-      <c r="C59" s="22">
+      <c r="C59" s="24">
         <f t="shared" ref="C59:F59" si="26">ABS((C16-C38)/C16)</f>
         <v>6.9999999999999923E-2</v>
       </c>
-      <c r="D59" s="22">
+      <c r="D59" s="24">
         <f t="shared" si="26"/>
         <v>0.23461538461538467</v>
       </c>
-      <c r="E59" s="22">
+      <c r="E59" s="24">
         <f t="shared" si="26"/>
         <v>0.69166666666666676</v>
       </c>
-      <c r="F59" s="22">
+      <c r="F59" s="24">
         <f t="shared" si="26"/>
         <v>8.1578947368421084E-2</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B60">
-        <f t="shared" ref="B60:F60" si="27">ABS((B17-B39)/B17)*100</f>
+      <c r="B60" s="23">
+        <f t="shared" ref="B60" si="27">ABS((B17-B39)/B17)*100</f>
         <v>0.14779235174579716</v>
       </c>
-      <c r="C60" s="22">
+      <c r="C60" s="24">
         <f t="shared" ref="C60:F60" si="28">ABS((C17-C39)/C17)</f>
         <v>1.2195121951219513E-2</v>
       </c>
-      <c r="D60" s="22">
+      <c r="D60" s="24">
         <f t="shared" si="28"/>
         <v>0.10100259933160044</v>
       </c>
-      <c r="E60" s="22">
+      <c r="E60" s="24">
         <f t="shared" si="28"/>
         <v>0.19016279875303083</v>
       </c>
-      <c r="F60" s="22">
+      <c r="F60" s="24">
         <f t="shared" si="28"/>
         <v>0.2430199900875599</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B61">
-        <f t="shared" ref="B61:F61" si="29">ABS((B18-B40)/B18)*100</f>
+      <c r="B61" s="23">
+        <f t="shared" ref="B61" si="29">ABS((B18-B40)/B18)*100</f>
         <v>4.5287637698898413</v>
       </c>
-      <c r="C61" s="22">
+      <c r="C61" s="24">
         <f t="shared" ref="C61:F61" si="30">ABS((C18-C40)/C18)</f>
         <v>4.528763769889841E-2</v>
       </c>
-      <c r="D61" s="22">
+      <c r="D61" s="24">
         <f t="shared" si="30"/>
         <v>4.4879640962872294E-2</v>
       </c>
-      <c r="E61" s="22">
+      <c r="E61" s="24">
         <f t="shared" si="30"/>
         <v>3.8950389503895039E-2</v>
       </c>
-      <c r="F61" s="22">
+      <c r="F61" s="24">
         <f t="shared" si="30"/>
         <v>0.18628246753246752</v>
       </c>
     </row>
     <row r="62" spans="1:18" ht="45.75" thickBot="1">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B62">
-        <f t="shared" ref="B62:F62" si="31">ABS((B19-B41)/B19)*100</f>
+      <c r="B62" s="23">
+        <f t="shared" ref="B62" si="31">ABS((B19-B41)/B19)*100</f>
         <v>4.0175557056043214</v>
       </c>
-      <c r="C62" s="22">
+      <c r="C62" s="24">
         <f t="shared" ref="C62:F62" si="32">ABS((C19-C41)/C19)</f>
         <v>5.9439378588314759E-2</v>
       </c>
-      <c r="D62" s="22">
+      <c r="D62" s="24">
         <f t="shared" si="32"/>
         <v>0.22282793867120954</v>
       </c>
-      <c r="E62" s="22">
+      <c r="E62" s="24">
         <f t="shared" si="32"/>
         <v>0.35731414868105515</v>
       </c>
-      <c r="F62" s="22">
+      <c r="F62" s="24">
         <f t="shared" si="32"/>
         <v>0.28161559888579385</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="30.75" thickBot="1">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B63">
-        <f t="shared" ref="B63:F63" si="33">ABS((B20-B42)/B20)*100</f>
+      <c r="B63" s="23">
+        <f t="shared" ref="B63" si="33">ABS((B20-B42)/B20)*100</f>
         <v>4.4444444444444446</v>
       </c>
-      <c r="C63" s="22">
+      <c r="C63" s="24">
         <f t="shared" ref="C63:F63" si="34">ABS((C20-C42)/C20)</f>
         <v>4.4444444444444446E-2</v>
       </c>
-      <c r="D63" s="22">
+      <c r="D63" s="24">
         <f t="shared" si="34"/>
         <v>0.15217391304347827</v>
       </c>
-      <c r="E63" s="22">
+      <c r="E63" s="24">
         <f t="shared" si="34"/>
         <v>0.19047619047619047</v>
       </c>
-      <c r="F63" s="22">
+      <c r="F63" s="24">
         <f t="shared" si="34"/>
         <v>4.878048780487805E-2</v>
       </c>
@@ -2546,23 +2492,23 @@
     <mergeCell ref="H32:L33"/>
   </mergeCells>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:F63">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>

</xml_diff>